<commit_message>
Added 2023 Saltmarsh Data
- Added 2023 Saltmarsh data
- Fixed bug in values graph where values were displaying incorrectly
- Added east trinity Shapefiles for NDVI Code
- Added datacube config file
- Added dummy photo for photo testing in Map_Test.py
</commit_message>
<xml_diff>
--- a/data/data_2024.xlsx
+++ b/data/data_2024.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LucanSinclair\OneDrive - Earthwatch\Desktop\Code\Earthwatch_Code\Saltmarsh-Savers\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4125EE99-0E7A-47A7-9E01-5E7A891D6E76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{C446CC89-77AC-4701-8892-154BBCFD41B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="12220" activeTab="1" xr2:uid="{EDC8C2C9-AF13-4847-9081-A01FE46671A3}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" activeTab="5" xr2:uid="{EDC8C2C9-AF13-4847-9081-A01FE46671A3}"/>
   </bookViews>
   <sheets>
     <sheet name="Machans Beach (Silver Site)" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="916" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="72">
   <si>
     <t>Threat</t>
   </si>
@@ -251,6 +251,9 @@
   </si>
   <si>
     <t>TVR</t>
+  </si>
+  <si>
+    <t>B</t>
   </si>
 </sst>
 </file>
@@ -1189,8 +1192,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9722E1D5-4268-4CFB-95A7-B673FD76448D}">
   <dimension ref="A1:L46"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1249,7 +1252,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>
@@ -1287,7 +1290,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>58</v>
@@ -1313,7 +1316,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>58</v>
@@ -1339,7 +1342,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>58</v>
@@ -1365,7 +1368,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -1391,7 +1394,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>58</v>
@@ -1417,7 +1420,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>59</v>
@@ -1443,7 +1446,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>59</v>
@@ -1469,7 +1472,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>59</v>
@@ -1495,7 +1498,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>58</v>
@@ -1521,7 +1524,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>58</v>
@@ -1547,7 +1550,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>58</v>
@@ -1573,7 +1576,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>58</v>
@@ -1599,7 +1602,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>58</v>
@@ -1625,7 +1628,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>58</v>
@@ -1651,7 +1654,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>58</v>
@@ -1677,7 +1680,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>58</v>
@@ -1703,7 +1706,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>58</v>
@@ -1729,7 +1732,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>59</v>
@@ -1755,7 +1758,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>59</v>
@@ -1781,7 +1784,7 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>59</v>
@@ -1807,7 +1810,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>58</v>
@@ -1833,16 +1836,13 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D24">
         <v>3.3505154639175259</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="25" spans="1:8">
@@ -1967,8 +1967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31F1C509-2F6E-4297-954C-B4FD037FDF3D}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2024,7 +2024,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>
@@ -2062,7 +2062,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>58</v>
@@ -2088,7 +2088,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>58</v>
@@ -2114,7 +2114,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>58</v>
@@ -2140,7 +2140,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -2166,7 +2166,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>58</v>
@@ -2192,7 +2192,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>59</v>
@@ -2218,7 +2218,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>59</v>
@@ -2244,7 +2244,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>59</v>
@@ -2270,7 +2270,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>58</v>
@@ -2296,7 +2296,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>58</v>
@@ -2322,7 +2322,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>58</v>
@@ -2348,7 +2348,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>58</v>
@@ -2374,7 +2374,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>58</v>
@@ -2400,7 +2400,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>58</v>
@@ -2426,7 +2426,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>58</v>
@@ -2452,7 +2452,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>58</v>
@@ -2478,7 +2478,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>58</v>
@@ -2504,7 +2504,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>59</v>
@@ -2530,7 +2530,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>59</v>
@@ -2556,7 +2556,7 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>59</v>
@@ -2582,7 +2582,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>58</v>
@@ -2608,16 +2608,13 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D24">
         <v>3.1754032258064515</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -2629,8 +2626,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9032AAA6-CDEB-4ECA-BC3D-9AB05617C8E9}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1:L2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -2689,7 +2686,7 @@
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>
@@ -2727,7 +2724,7 @@
         <v>13</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>58</v>
@@ -2753,7 +2750,7 @@
         <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>58</v>
@@ -2779,7 +2776,7 @@
         <v>15</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>58</v>
@@ -2805,7 +2802,7 @@
         <v>17</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -2831,7 +2828,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>58</v>
@@ -2857,7 +2854,7 @@
         <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>58</v>
@@ -2883,7 +2880,7 @@
         <v>19</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>58</v>
@@ -2909,7 +2906,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>58</v>
@@ -2935,7 +2932,7 @@
         <v>23</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>58</v>
@@ -2961,7 +2958,7 @@
         <v>27</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>58</v>
@@ -2987,7 +2984,7 @@
         <v>37</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>58</v>
@@ -3013,7 +3010,7 @@
         <v>31</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>58</v>
@@ -3039,7 +3036,7 @@
         <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>58</v>
@@ -3065,7 +3062,7 @@
         <v>33</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>58</v>
@@ -3091,7 +3088,7 @@
         <v>35</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>58</v>
@@ -3117,7 +3114,7 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>59</v>
@@ -3143,7 +3140,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>59</v>
@@ -3169,7 +3166,7 @@
         <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>59</v>
@@ -3195,7 +3192,7 @@
         <v>41</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>59</v>
@@ -3221,7 +3218,7 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>59</v>
@@ -3247,7 +3244,7 @@
         <v>47</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>59</v>
@@ -3273,16 +3270,13 @@
         <v>51</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D24">
         <v>0.58207217694994184</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3297,8 +3291,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{68A37732-9494-4BA2-8F38-96E03CDFAC84}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="L9" sqref="L9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -3353,7 +3347,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>
@@ -3391,7 +3385,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>58</v>
@@ -3417,7 +3411,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>58</v>
@@ -3443,7 +3437,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>58</v>
@@ -3469,7 +3463,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -3495,7 +3489,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>58</v>
@@ -3521,7 +3515,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>59</v>
@@ -3547,7 +3541,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>59</v>
@@ -3573,7 +3567,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>59</v>
@@ -3599,7 +3593,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>58</v>
@@ -3625,7 +3619,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>58</v>
@@ -3651,7 +3645,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>58</v>
@@ -3677,7 +3671,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>58</v>
@@ -3703,7 +3697,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>58</v>
@@ -3729,7 +3723,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>58</v>
@@ -3755,7 +3749,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>58</v>
@@ -3781,7 +3775,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>58</v>
@@ -3807,7 +3801,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>58</v>
@@ -3833,7 +3827,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>59</v>
@@ -3859,7 +3853,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>59</v>
@@ -3885,7 +3879,7 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>59</v>
@@ -3911,7 +3905,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>58</v>
@@ -3937,16 +3931,13 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D24">
         <v>0</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -3958,8 +3949,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F84A2B-CB62-41C5-91B0-5634E1251A98}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4014,7 +4005,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>
@@ -4052,7 +4043,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>58</v>
@@ -4078,7 +4069,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>58</v>
@@ -4104,7 +4095,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>58</v>
@@ -4130,7 +4121,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -4156,7 +4147,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>58</v>
@@ -4182,7 +4173,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>59</v>
@@ -4208,7 +4199,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>59</v>
@@ -4234,7 +4225,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>59</v>
@@ -4260,7 +4251,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>58</v>
@@ -4286,7 +4277,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>58</v>
@@ -4312,7 +4303,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>58</v>
@@ -4338,7 +4329,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>58</v>
@@ -4364,7 +4355,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>58</v>
@@ -4390,7 +4381,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>58</v>
@@ -4416,7 +4407,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>58</v>
@@ -4442,7 +4433,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>58</v>
@@ -4468,7 +4459,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>58</v>
@@ -4494,7 +4485,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>59</v>
@@ -4520,7 +4511,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>59</v>
@@ -4546,7 +4537,7 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>59</v>
@@ -4572,7 +4563,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>58</v>
@@ -4598,16 +4589,13 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D24">
         <v>0.78695896571107371</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>
@@ -4619,8 +4607,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9047EB6-D702-48A6-8501-7AF99B0EA744}">
   <dimension ref="A1:L24"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -4675,7 +4663,7 @@
         <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C2" s="12" t="s">
         <v>58</v>
@@ -4713,7 +4701,7 @@
         <v>33</v>
       </c>
       <c r="B3" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C3" s="12" t="s">
         <v>58</v>
@@ -4739,7 +4727,7 @@
         <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C4" s="12" t="s">
         <v>58</v>
@@ -4765,7 +4753,7 @@
         <v>35</v>
       </c>
       <c r="B5" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C5" s="12" t="s">
         <v>58</v>
@@ -4791,7 +4779,7 @@
         <v>37</v>
       </c>
       <c r="B6" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
         <v>58</v>
@@ -4817,7 +4805,7 @@
         <v>25</v>
       </c>
       <c r="B7" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C7" s="12" t="s">
         <v>58</v>
@@ -4843,7 +4831,7 @@
         <v>49</v>
       </c>
       <c r="B8" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C8" s="12" t="s">
         <v>59</v>
@@ -4869,7 +4857,7 @@
         <v>41</v>
       </c>
       <c r="B9" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C9" s="12" t="s">
         <v>59</v>
@@ -4895,7 +4883,7 @@
         <v>51</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C10" s="12" t="s">
         <v>59</v>
@@ -4921,7 +4909,7 @@
         <v>21</v>
       </c>
       <c r="B11" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C11" s="12" t="s">
         <v>58</v>
@@ -4947,7 +4935,7 @@
         <v>19</v>
       </c>
       <c r="B12" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C12" s="12" t="s">
         <v>58</v>
@@ -4973,7 +4961,7 @@
         <v>9</v>
       </c>
       <c r="B13" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>58</v>
@@ -4999,7 +4987,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>58</v>
@@ -5025,7 +5013,7 @@
         <v>27</v>
       </c>
       <c r="B15" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C15" s="12" t="s">
         <v>58</v>
@@ -5051,7 +5039,7 @@
         <v>17</v>
       </c>
       <c r="B16" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C16" s="12" t="s">
         <v>58</v>
@@ -5077,7 +5065,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C17" s="12" t="s">
         <v>58</v>
@@ -5103,7 +5091,7 @@
         <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C18" s="12" t="s">
         <v>58</v>
@@ -5129,7 +5117,7 @@
         <v>6</v>
       </c>
       <c r="B19" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C19" s="12" t="s">
         <v>58</v>
@@ -5155,7 +5143,7 @@
         <v>39</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C20" s="12" t="s">
         <v>59</v>
@@ -5181,7 +5169,7 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C21" s="12" t="s">
         <v>59</v>
@@ -5207,7 +5195,7 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C22" s="12" t="s">
         <v>59</v>
@@ -5233,7 +5221,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C23" s="12" t="s">
         <v>58</v>
@@ -5259,16 +5247,13 @@
         <v>47</v>
       </c>
       <c r="B24" t="s">
-        <v>60</v>
+        <v>71</v>
       </c>
       <c r="C24" s="12" t="s">
         <v>59</v>
       </c>
       <c r="D24">
         <v>0.76738609112709832</v>
-      </c>
-      <c r="F24" t="s">
-        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>